<commit_message>
working on KTR Manager, right now new teamples are created and stored both on the disk and the location to the template is stored in the db in the new table SourceInfoTableKTR, refs #338
</commit_message>
<xml_diff>
--- a/src/test/resources/testExcelFile.xlsx
+++ b/src/test/resources/testExcelFile.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13700" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13700" windowHeight="17480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>A</t>
   </si>
@@ -46,6 +47,30 @@
   </si>
   <si>
     <t>3cc</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>d1</t>
+  </si>
+  <si>
+    <t>e1</t>
+  </si>
+  <si>
+    <t>d2</t>
+  </si>
+  <si>
+    <t>e2</t>
+  </si>
+  <si>
+    <t>d3</t>
+  </si>
+  <si>
+    <t>e3</t>
   </si>
 </sst>
 </file>
@@ -452,7 +477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -511,4 +536,56 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>